<commit_message>
finished preliminary effectiveness calculations. toma epidemiologos!
</commit_message>
<xml_diff>
--- a/public_data/parameters.xlsx
+++ b/public_data/parameters.xlsx
@@ -15,40 +15,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-we only have information disagregated by age for those under 15….(see Quique's paper)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
@@ -101,36 +67,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -156,41 +99,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -488,249 +420,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="6" customWidth="1"/>
-    <col min="3" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="14.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="24.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="3" customWidth="1"/>
+    <col min="3" max="8" width="14.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="5">
         <v>0.73</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>0.27</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>0.27</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="5">
         <v>1.71</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="5">
         <v>108.02</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="5">
         <v>36820</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="5">
         <v>10809</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <v>6000</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="5">
         <v>16401</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>35799</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="5">
         <v>44848</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>28713</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>